<commit_message>
Step 4: Added all the required values into the test plan.
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\8. Activities\Module_01\given_files\activity_1\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RRC_polytech\Term2\IntSoftwareDev\Module1\Assignments\comp-2327-activity-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94801D8B-F184-4C7C-AC17-1E2ABA18B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3560184F-5543-4935-B267-F5A917665221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,6 +249,48 @@
   </si>
   <si>
     <t>Attribute  set to input values.</t>
+  </si>
+  <si>
+    <t>Hudson Drozdowski</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>title = "Book Name"                                                author = "Author Name"                                       genre = FICTION</t>
+  </si>
+  <si>
+    <t>The instnace is inititalized correctly, no errors.</t>
+  </si>
+  <si>
+    <t>ValueError("Title cannot be blank.")</t>
+  </si>
+  <si>
+    <t>raise ValueError("Author cannot be blank.")</t>
+  </si>
+  <si>
+    <t>title = "Book Name"                                                                                     author = ""                                                         genre = TRUE_CRIME</t>
+  </si>
+  <si>
+    <t>title = ""                                                                                     author = "Author Name"                                         genre = NON_FICTION</t>
+  </si>
+  <si>
+    <t>title = "Book Name"                                                                                     author = "Author Name"                                         genre = RANDOM_GENRE</t>
+  </si>
+  <si>
+    <t>ValueError("Invalid Genre")</t>
+  </si>
+  <si>
+    <t>The object is initialized correctly     title = "Book Name"                                                author = "Author Name"                                       genre = FICTION</t>
+  </si>
+  <si>
+    <t>"Book Name"</t>
+  </si>
+  <si>
+    <t>"Author Name"</t>
+  </si>
+  <si>
+    <t>FICTION</t>
   </si>
 </sst>
 </file>
@@ -1109,22 +1151,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:7" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="1.8">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1136,14 +1178,16 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1152,10 +1196,10 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1186,11 +1230,17 @@
       <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1201,11 +1251,17 @@
       <c r="D8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="12">
         <v>3</v>
@@ -1216,11 +1272,17 @@
       <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="11">
         <v>4</v>
@@ -1231,11 +1293,17 @@
       <c r="D10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12">
         <v>5</v>
       </c>
@@ -1245,11 +1313,15 @@
       <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -1259,11 +1331,15 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11">
         <v>7</v>
       </c>
@@ -1273,11 +1349,15 @@
       <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>10</v>
       </c>
@@ -1287,7 +1367,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12">
         <v>11</v>
       </c>
@@ -1297,7 +1377,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12">
         <v>12</v>
       </c>
@@ -1307,7 +1387,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="11">
         <v>13</v>
       </c>
@@ -1317,7 +1397,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
         <v>14</v>
       </c>
@@ -1327,7 +1407,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
         <v>15</v>
       </c>
@@ -1337,7 +1417,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
         <v>16</v>
       </c>
@@ -1347,7 +1427,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
         <v>17</v>
       </c>
@@ -1357,7 +1437,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="12">
         <v>18</v>
       </c>
@@ -1367,7 +1447,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11">
         <v>19</v>
       </c>
@@ -1377,7 +1457,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12">
         <v>20</v>
       </c>
@@ -1387,7 +1467,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="19" t="s">
         <v>6</v>
       </c>
@@ -1413,6 +1493,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B3B6B51C940774DBF92367B1D1A75F0" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="80d4f13eaa95653e2ff902bb880fefc3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee0e594b-5dc6-49aa-9be8-f17bb89b127c" xmlns:ns3="b80edf0c-bd47-4bae-8c19-89fc2af9398f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ababe2f621e4b192c84b1cec6edec4f" ns2:_="" ns3:_="">
     <xsd:import namespace="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
@@ -1607,15 +1696,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1628,13 +1708,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37F01E9C-39D8-491B-950E-769C54FF39B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37F01E9C-39D8-491B-950E-769C54FF39B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Part 2 Step 3: Updated the test plan to have the correct values for the new tests
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RRC_polytech\Term2\IntSoftwareDev\Module1\Assignments\comp-2327-activity-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3560184F-5543-4935-B267-F5A917665221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF810C7D-5885-4ECE-BD3B-4C6075A66728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="47">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -257,9 +257,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>title = "Book Name"                                                author = "Author Name"                                       genre = FICTION</t>
-  </si>
-  <si>
     <t>The instnace is inititalized correctly, no errors.</t>
   </si>
   <si>
@@ -269,15 +266,6 @@
     <t>raise ValueError("Author cannot be blank.")</t>
   </si>
   <si>
-    <t>title = "Book Name"                                                                                     author = ""                                                         genre = TRUE_CRIME</t>
-  </si>
-  <si>
-    <t>title = ""                                                                                     author = "Author Name"                                         genre = NON_FICTION</t>
-  </si>
-  <si>
-    <t>title = "Book Name"                                                                                     author = "Author Name"                                         genre = RANDOM_GENRE</t>
-  </si>
-  <si>
     <t>ValueError("Invalid Genre")</t>
   </si>
   <si>
@@ -290,7 +278,52 @@
     <t>"Author Name"</t>
   </si>
   <si>
-    <t>FICTION</t>
+    <t>genre.FICTION</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>returns the item id</t>
+  </si>
+  <si>
+    <t>is_barrowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">returns true or false </t>
+  </si>
+  <si>
+    <t>exception raised when item_id is not a int</t>
+  </si>
+  <si>
+    <t>exception raised when is_barrowed is not a bool</t>
+  </si>
+  <si>
+    <t>ValueError("Is Borrowed must be a boolean value.")</t>
+  </si>
+  <si>
+    <t>title = "Book Name"                                                author = "Author Name"                                       genre = FICTION                                                               item_id = 1                                                                               is_borrowed = "Invalid input"</t>
+  </si>
+  <si>
+    <t>The object is initialized correctly     title = "Book Name"                                                author = "Author Name"                                       genre = FICTION                                                  item_id = 1                                                               is_borrowed = true</t>
+  </si>
+  <si>
+    <t>title = "Book Name"                                                author = "Author Name"                                       genre = FICTION                                                               item_id = "Invalid input"                                                                               is_borrowed = true</t>
+  </si>
+  <si>
+    <t>title = "Book Name"                                                                                     author = "Author Name"                                         genre = "This is wrong"                                             item_id = 1                                                                               is_borrowed = true</t>
+  </si>
+  <si>
+    <t>title = "Book Name"                                                                                     author = ""                                                         genre = TRUE_CRIME                                                             item_id = 1                                                                               is_borrowed = true</t>
+  </si>
+  <si>
+    <t>title = ""                                                                                     author = "Author Name"                                         genre = NON_FICTION                                                       item_id = 1                                                                               is_borrowed = true</t>
+  </si>
+  <si>
+    <t>title = "Book Name"                                                author = "Author Name"                                       genre = FICTION                                                               item_id = 1                                                                               is_borrowed = true</t>
+  </si>
+  <si>
+    <t>ValueError("Item Id must be numeric.")</t>
   </si>
 </sst>
 </file>
@@ -545,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -594,6 +627,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1151,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,7 +1255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="11">
         <v>1</v>
@@ -1234,13 +1270,13 @@
         <v>23</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="12">
         <v>2</v>
@@ -1255,10 +1291,10 @@
         <v>23</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1276,10 +1312,10 @@
         <v>23</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1297,10 +1333,10 @@
         <v>23</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.3">
@@ -1314,11 +1350,13 @@
         <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="G11" s="9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1332,11 +1370,13 @@
         <v>18</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="9"/>
+        <v>28</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="G12" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1350,56 +1390,98 @@
         <v>19</v>
       </c>
       <c r="E13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="11">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9" t="s">
+      <c r="D14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B15" s="12">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11">
+      <c r="E15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B16" s="12">
         <v>10</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="12">
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B17" s="11">
         <v>11</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="12">
-        <v>12</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11">
-        <v>13</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1409,7 +1491,7 @@
     </row>
     <row r="19" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="12">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1419,7 +1501,7 @@
     </row>
     <row r="20" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1429,7 +1511,7 @@
     </row>
     <row r="21" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="12">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1439,7 +1521,7 @@
     </row>
     <row r="22" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="12">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1449,7 +1531,7 @@
     </row>
     <row r="23" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -1459,7 +1541,7 @@
     </row>
     <row r="24" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="12">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -1485,20 +1567,23 @@
     <mergeCell ref="B26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee0e594b-5dc6-49aa-9be8-f17bb89b127c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b80edf0c-bd47-4bae-8c19-89fc2af9398f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1697,20 +1782,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee0e594b-5dc6-49aa-9be8-f17bb89b127c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b80edf0c-bd47-4bae-8c19-89fc2af9398f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1735,12 +1821,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
-    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix: fixed the instanceing test to include item_id, & is_borrowed.
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RRC_polytech\Term2\IntSoftwareDev\Module1\Assignments\comp-2327-activity-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF810C7D-5885-4ECE-BD3B-4C6075A66728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71DA9AD-2F1B-48B1-9979-D8BC80812D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -604,6 +604,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -627,9 +630,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,31 +1206,31 @@
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -1415,7 +1415,7 @@
       <c r="F14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="13">
         <v>1</v>
       </c>
     </row>
@@ -1435,7 +1435,7 @@
       <c r="F15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="21" t="b">
+      <c r="G15" s="13" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1550,14 +1550,14 @@
       <c r="G24" s="3"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1576,14 +1576,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee0e594b-5dc6-49aa-9be8-f17bb89b127c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b80edf0c-bd47-4bae-8c19-89fc2af9398f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1782,21 +1780,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee0e594b-5dc6-49aa-9be8-f17bb89b127c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b80edf0c-bd47-4bae-8c19-89fc2af9398f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
-    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1821,9 +1818,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3194B8C0-471E-4E12-8338-7B9268783B6C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93494D4A-B25F-4AE9-9242-3524F3518EDF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ee0e594b-5dc6-49aa-9be8-f17bb89b127c"/>
+    <ds:schemaRef ds:uri="b80edf0c-bd47-4bae-8c19-89fc2af9398f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>